<commit_message>
Add folder of app
</commit_message>
<xml_diff>
--- a/Check.xlsx
+++ b/Check.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" refMode="R1C1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -1166,7 +1166,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1235,7 +1235,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -1557,8 +1556,8 @@
   <sheetPr codeName="Лист1"/>
   <dimension ref="A1:J92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="0">
-      <selection activeCell="E93" sqref="E93"/>
+    <sheetView tabSelected="1" topLeftCell="A86" workbookViewId="0">
+      <selection activeCell="E96" sqref="E96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -3558,7 +3557,7 @@
       <c r="D88" s="5">
         <v>87</v>
       </c>
-      <c r="E88" s="24" t="s">
+      <c r="E88" s="6" t="s">
         <v>142</v>
       </c>
       <c r="F88" s="7" t="s">
@@ -3581,7 +3580,7 @@
       <c r="D89" s="5">
         <v>88</v>
       </c>
-      <c r="E89" s="24" t="s">
+      <c r="E89" s="6" t="s">
         <v>143</v>
       </c>
       <c r="F89" s="7" t="s">
@@ -3604,7 +3603,7 @@
       <c r="D90" s="5">
         <v>89</v>
       </c>
-      <c r="E90" s="24" t="s">
+      <c r="E90" s="6" t="s">
         <v>144</v>
       </c>
       <c r="F90" s="7" t="s">
@@ -3627,7 +3626,7 @@
       <c r="D91" s="5">
         <v>90</v>
       </c>
-      <c r="E91" s="24" t="s">
+      <c r="E91" s="6" t="s">
         <v>145</v>
       </c>
       <c r="F91" s="7" t="s">
@@ -3650,7 +3649,7 @@
       <c r="D92" s="5">
         <v>91</v>
       </c>
-      <c r="E92" s="24" t="s">
+      <c r="E92" s="6" t="s">
         <v>146</v>
       </c>
       <c r="F92" s="7" t="s">

</xml_diff>